<commit_message>
mici modificari si 2 rulari pe laptop
</commit_message>
<xml_diff>
--- a/prod.xlsx
+++ b/prod.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -435,13 +435,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FZ2"/>
+  <dimension ref="A1:FZ4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -2262,6 +2265,1810 @@
         </is>
       </c>
       <c r="FZ2" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>19/02/2023 17:26:52</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>2845</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>1267</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>88</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>289</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>917</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AL3" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="AM3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AN3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AO3" t="inlineStr">
+        <is>
+          <t>6399</t>
+        </is>
+      </c>
+      <c r="AP3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AQ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AR3" t="inlineStr">
+        <is>
+          <t>3183</t>
+        </is>
+      </c>
+      <c r="AS3" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AT3" t="inlineStr">
+        <is>
+          <t>3120</t>
+        </is>
+      </c>
+      <c r="AU3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AV3" t="inlineStr">
+        <is>
+          <t>2322</t>
+        </is>
+      </c>
+      <c r="AW3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AX3" t="inlineStr">
+        <is>
+          <t>1652</t>
+        </is>
+      </c>
+      <c r="AY3" t="inlineStr">
+        <is>
+          <t>4007</t>
+        </is>
+      </c>
+      <c r="AZ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BA3" t="inlineStr">
+        <is>
+          <t>2644</t>
+        </is>
+      </c>
+      <c r="BB3" t="inlineStr">
+        <is>
+          <t>2100</t>
+        </is>
+      </c>
+      <c r="BC3" t="inlineStr">
+        <is>
+          <t>8156</t>
+        </is>
+      </c>
+      <c r="BD3" t="inlineStr">
+        <is>
+          <t>9637</t>
+        </is>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>3708</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>1845</t>
+        </is>
+      </c>
+      <c r="BG3" t="inlineStr">
+        <is>
+          <t>5200</t>
+        </is>
+      </c>
+      <c r="BH3" t="inlineStr">
+        <is>
+          <t>263</t>
+        </is>
+      </c>
+      <c r="BI3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BJ3" t="inlineStr">
+        <is>
+          <t>2508</t>
+        </is>
+      </c>
+      <c r="BK3" t="inlineStr">
+        <is>
+          <t>11088</t>
+        </is>
+      </c>
+      <c r="BL3" t="inlineStr">
+        <is>
+          <t>5838</t>
+        </is>
+      </c>
+      <c r="BM3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BN3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="BO3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BP3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BQ3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BR3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BS3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BT3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BU3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="BV3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BW3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="BX3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BY3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BZ3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CA3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CB3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CC3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CD3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CE3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CF3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CG3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CH3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CI3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CJ3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CK3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CN3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CO3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CP3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="CQ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CR3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CS3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CT3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CU3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CV3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CW3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CX3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CY3" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="CZ3" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="DA3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="DB3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="DC3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="DD3" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="DE3" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="DF3" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="DG3" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="DH3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="DI3" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="DJ3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="DK3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="DL3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="DM3" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="DN3" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="DO3" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="DP3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="DQ3" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="DR3" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="DS3" t="inlineStr">
+        <is>
+          <t>5518</t>
+        </is>
+      </c>
+      <c r="DT3" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="DU3" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="DV3" t="inlineStr">
+        <is>
+          <t>403</t>
+        </is>
+      </c>
+      <c r="DW3" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="DX3" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="DY3" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
+      </c>
+      <c r="DZ3" t="inlineStr">
+        <is>
+          <t>344</t>
+        </is>
+      </c>
+      <c r="EA3" t="inlineStr">
+        <is>
+          <t>333</t>
+        </is>
+      </c>
+      <c r="EB3" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="EC3" t="inlineStr">
+        <is>
+          <t>470</t>
+        </is>
+      </c>
+      <c r="ED3" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="EE3" t="inlineStr">
+        <is>
+          <t>526</t>
+        </is>
+      </c>
+      <c r="EF3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EG3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EH3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EI3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EJ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EK3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EL3" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="EM3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EN3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EO3" t="inlineStr">
+        <is>
+          <t>312</t>
+        </is>
+      </c>
+      <c r="EP3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EQ3" t="inlineStr">
+        <is>
+          <t>2931</t>
+        </is>
+      </c>
+      <c r="ER3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="ES3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="ET3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="EU3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="EV3" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="EW3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EX3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EY3" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="EZ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FA3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FB3" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="FC3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FD3" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+      <c r="FE3" t="inlineStr">
+        <is>
+          <t>4453</t>
+        </is>
+      </c>
+      <c r="FF3" t="inlineStr">
+        <is>
+          <t>3770</t>
+        </is>
+      </c>
+      <c r="FG3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FH3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FI3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FJ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FK3" t="inlineStr">
+        <is>
+          <t>3975</t>
+        </is>
+      </c>
+      <c r="FL3" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="FM3" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="FN3" t="inlineStr">
+        <is>
+          <t>1313</t>
+        </is>
+      </c>
+      <c r="FO3" t="inlineStr">
+        <is>
+          <t>615</t>
+        </is>
+      </c>
+      <c r="FP3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FQ3" t="inlineStr">
+        <is>
+          <t>1147</t>
+        </is>
+      </c>
+      <c r="FR3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FS3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FT3" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="FU3" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="FV3" t="inlineStr">
+        <is>
+          <t>261</t>
+        </is>
+      </c>
+      <c r="FW3" t="inlineStr">
+        <is>
+          <t>269</t>
+        </is>
+      </c>
+      <c r="FX3" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="FY3" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="FZ3" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20/02/2023 19:32:02</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>2828</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>1257</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>286</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>905</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AL4" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="AM4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AN4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>6399</t>
+        </is>
+      </c>
+      <c r="AP4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AQ4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AR4" t="inlineStr">
+        <is>
+          <t>3183</t>
+        </is>
+      </c>
+      <c r="AS4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="AT4" t="inlineStr">
+        <is>
+          <t>3117</t>
+        </is>
+      </c>
+      <c r="AU4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AV4" t="inlineStr">
+        <is>
+          <t>2171</t>
+        </is>
+      </c>
+      <c r="AW4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="AX4" t="inlineStr">
+        <is>
+          <t>1446</t>
+        </is>
+      </c>
+      <c r="AY4" t="inlineStr">
+        <is>
+          <t>3845</t>
+        </is>
+      </c>
+      <c r="AZ4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BA4" t="inlineStr">
+        <is>
+          <t>2643</t>
+        </is>
+      </c>
+      <c r="BB4" t="inlineStr">
+        <is>
+          <t>2100</t>
+        </is>
+      </c>
+      <c r="BC4" t="inlineStr">
+        <is>
+          <t>7486</t>
+        </is>
+      </c>
+      <c r="BD4" t="inlineStr">
+        <is>
+          <t>9545</t>
+        </is>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>3654</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>1844</t>
+        </is>
+      </c>
+      <c r="BG4" t="inlineStr">
+        <is>
+          <t>4857</t>
+        </is>
+      </c>
+      <c r="BH4" t="inlineStr">
+        <is>
+          <t>251</t>
+        </is>
+      </c>
+      <c r="BI4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BJ4" t="inlineStr">
+        <is>
+          <t>2452</t>
+        </is>
+      </c>
+      <c r="BK4" t="inlineStr">
+        <is>
+          <t>10925</t>
+        </is>
+      </c>
+      <c r="BL4" t="inlineStr">
+        <is>
+          <t>5837</t>
+        </is>
+      </c>
+      <c r="BM4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BN4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="BO4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BP4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BQ4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BR4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BS4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="BT4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BU4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="BV4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BW4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BX4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BY4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="BZ4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CA4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CB4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CC4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CD4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CE4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CF4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CG4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CH4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CI4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CJ4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CK4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CN4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CO4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CP4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="CQ4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CR4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CS4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CT4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CU4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="CV4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="CW4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="CX4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="CY4" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="CZ4" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="DA4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="DB4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="DC4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="DD4" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="DE4" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="DF4" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="DG4" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="DH4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="DI4" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="DJ4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="DK4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="DL4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="DM4" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="DN4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="DO4" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="DP4" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="DQ4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="DR4" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="DS4" t="inlineStr">
+        <is>
+          <t>5451</t>
+        </is>
+      </c>
+      <c r="DT4" t="inlineStr">
+        <is>
+          <t>84</t>
+        </is>
+      </c>
+      <c r="DU4" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="DV4" t="inlineStr">
+        <is>
+          <t>403</t>
+        </is>
+      </c>
+      <c r="DW4" t="inlineStr">
+        <is>
+          <t>219</t>
+        </is>
+      </c>
+      <c r="DX4" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="DY4" t="inlineStr">
+        <is>
+          <t>339</t>
+        </is>
+      </c>
+      <c r="DZ4" t="inlineStr">
+        <is>
+          <t>343</t>
+        </is>
+      </c>
+      <c r="EA4" t="inlineStr">
+        <is>
+          <t>329</t>
+        </is>
+      </c>
+      <c r="EB4" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="EC4" t="inlineStr">
+        <is>
+          <t>469</t>
+        </is>
+      </c>
+      <c r="ED4" t="inlineStr">
+        <is>
+          <t>583</t>
+        </is>
+      </c>
+      <c r="EE4" t="inlineStr">
+        <is>
+          <t>498</t>
+        </is>
+      </c>
+      <c r="EF4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EG4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EH4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EI4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EJ4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EK4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EL4" t="inlineStr">
+        <is>
+          <t>86</t>
+        </is>
+      </c>
+      <c r="EM4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EN4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EO4" t="inlineStr">
+        <is>
+          <t>311</t>
+        </is>
+      </c>
+      <c r="EP4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EQ4" t="inlineStr">
+        <is>
+          <t>2931</t>
+        </is>
+      </c>
+      <c r="ER4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="ES4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="ET4" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="EU4" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="EV4" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="EW4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EX4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="EY4" t="inlineStr">
+        <is>
+          <t>87</t>
+        </is>
+      </c>
+      <c r="EZ4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FA4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FB4" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="FC4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FD4" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+      <c r="FE4" t="inlineStr">
+        <is>
+          <t>4453</t>
+        </is>
+      </c>
+      <c r="FF4" t="inlineStr">
+        <is>
+          <t>3770</t>
+        </is>
+      </c>
+      <c r="FG4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FH4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FI4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FJ4" t="inlineStr">
+        <is>
+          <t>146</t>
+        </is>
+      </c>
+      <c r="FK4" t="inlineStr">
+        <is>
+          <t>3975</t>
+        </is>
+      </c>
+      <c r="FL4" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="FM4" t="inlineStr">
+        <is>
+          <t>N\A MULTIPLE SELECTIONS AVAILABLE</t>
+        </is>
+      </c>
+      <c r="FN4" t="inlineStr">
+        <is>
+          <t>1213</t>
+        </is>
+      </c>
+      <c r="FO4" t="inlineStr">
+        <is>
+          <t>381</t>
+        </is>
+      </c>
+      <c r="FP4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FQ4" t="inlineStr">
+        <is>
+          <t>1147</t>
+        </is>
+      </c>
+      <c r="FR4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FS4" t="inlineStr">
+        <is>
+          <t>N\A</t>
+        </is>
+      </c>
+      <c r="FT4" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="FU4" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="FV4" t="inlineStr">
+        <is>
+          <t>261</t>
+        </is>
+      </c>
+      <c r="FW4" t="inlineStr">
+        <is>
+          <t>269</t>
+        </is>
+      </c>
+      <c r="FX4" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="FY4" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="FZ4" t="inlineStr">
         <is>
           <t>N\A</t>
         </is>

</xml_diff>